<commit_message>
Cheetah Men II - up to the end of the boss, but don't know how to finish!
</commit_message>
<xml_diff>
--- a/CheetahMenII/Cheetah Men II.xlsx
+++ b/CheetahMenII/Cheetah Men II.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="247">
   <si>
     <t>Notes</t>
   </si>
@@ -730,6 +730,66 @@
   <si>
     <t>X = 13 172</t>
   </si>
+  <si>
+    <t>X = 188</t>
+  </si>
+  <si>
+    <t>X = 3 192</t>
+  </si>
+  <si>
+    <t>X = 4 220</t>
+  </si>
+  <si>
+    <t>X = 5 220</t>
+  </si>
+  <si>
+    <t>X = 10 136</t>
+  </si>
+  <si>
+    <t>X = 6 004</t>
+  </si>
+  <si>
+    <t>X = 8 128</t>
+  </si>
+  <si>
+    <t>X = 8 60</t>
+  </si>
+  <si>
+    <t>X - 9 216</t>
+  </si>
+  <si>
+    <t>X = 10 244</t>
+  </si>
+  <si>
+    <t>X = 11 196</t>
+  </si>
+  <si>
+    <t>X = 11 200</t>
+  </si>
+  <si>
+    <t>X = 12 168</t>
+  </si>
+  <si>
+    <t>X = 12 200</t>
+  </si>
+  <si>
+    <t>X = 13 140</t>
+  </si>
+  <si>
+    <t>X = 13 180</t>
+  </si>
+  <si>
+    <t>X = 14 228</t>
+  </si>
+  <si>
+    <t>X = 15 188</t>
+  </si>
+  <si>
+    <t>X = 15 0 (End)</t>
+  </si>
+  <si>
+    <t>Boss Appears</t>
+  </si>
 </sst>
 </file>
 
@@ -739,10 +799,17 @@
     <numFmt numFmtId="164" formatCode="#,##0;[Red]#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="45" x14ac:knownFonts="1">
+  <fonts count="46" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1655,34 +1722,34 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="215">
+  <cellXfs count="216">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1690,208 +1757,208 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="23" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="25" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="26" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="27" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="26" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="26" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="26" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="26" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="27" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="27" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="27" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="27" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="27" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="28" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="26" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="29" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="27" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1901,10 +1968,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1925,141 +1992,144 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="43" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="44" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="44" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="43" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="35" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -2374,11 +2444,11 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:K68"/>
+  <dimension ref="A1:K94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
+      <pane ySplit="6" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -2394,20 +2464,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A1" s="154" t="s">
+      <c r="A1" s="156" t="s">
         <v>210</v>
       </c>
-      <c r="B1" s="153"/>
-      <c r="C1" s="155" t="s">
+      <c r="B1" s="155"/>
+      <c r="C1" s="157" t="s">
         <v>172</v>
       </c>
-      <c r="D1" s="155"/>
-      <c r="E1" s="155"/>
-      <c r="F1" s="156"/>
+      <c r="D1" s="157"/>
+      <c r="E1" s="157"/>
+      <c r="F1" s="158"/>
       <c r="G1" s="140"/>
       <c r="H1" s="141">
-        <f>SUM(G1:G65449)</f>
-        <v>0</v>
+        <f>SUM(G1:G65475)</f>
+        <v>8380</v>
       </c>
       <c r="I1" s="141" t="s">
         <v>199</v>
@@ -2429,19 +2499,19 @@
       <c r="G2" s="140"/>
       <c r="H2" s="144">
         <f>IF(H1&lt;3600,H1/60,QUOTIENT(H1, 3600))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I2" s="141" t="str">
         <f>IF(H1&lt;3600,"Seconds","Minutes")</f>
-        <v>Seconds</v>
-      </c>
-      <c r="J2" s="144" t="str">
+        <v>Minutes</v>
+      </c>
+      <c r="J2" s="144">
         <f>IF(H1&lt;3600,"",(MOD(H1,3600)/60))</f>
-        <v/>
+        <v>19.666666666666668</v>
       </c>
       <c r="K2" s="141" t="str">
         <f>IF(H1&lt;3600, "", "Seconds")</f>
-        <v/>
+        <v>Seconds</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2481,10 +2551,10 @@
       <c r="B5" s="147" t="s">
         <v>179</v>
       </c>
-      <c r="C5" s="152" t="s">
+      <c r="C5" s="154" t="s">
         <v>181</v>
       </c>
-      <c r="D5" s="152"/>
+      <c r="D5" s="154"/>
       <c r="E5" s="147"/>
       <c r="F5" s="143"/>
       <c r="G5" s="140"/>
@@ -2500,10 +2570,10 @@
       <c r="B6" s="147" t="s">
         <v>182</v>
       </c>
-      <c r="C6" s="152" t="s">
+      <c r="C6" s="154" t="s">
         <v>168</v>
       </c>
-      <c r="D6" s="153"/>
+      <c r="D6" s="155"/>
       <c r="E6" s="147"/>
       <c r="F6" s="143"/>
       <c r="G6" s="140"/>
@@ -2521,7 +2591,7 @@
       <c r="F7" s="93"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="157" t="s">
+      <c r="A8" s="159" t="s">
         <v>183</v>
       </c>
       <c r="B8" s="95" t="s">
@@ -2541,7 +2611,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="150"/>
+      <c r="A9" s="152"/>
       <c r="B9" s="98" t="s">
         <v>179</v>
       </c>
@@ -2555,7 +2625,7 @@
       <c r="F9" s="104"/>
     </row>
     <row r="10" spans="1:11" ht="12" customHeight="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="150"/>
+      <c r="A10" s="152"/>
       <c r="B10" s="148"/>
       <c r="C10" s="101"/>
       <c r="D10" s="101"/>
@@ -2566,7 +2636,7 @@
       <c r="F10" s="105"/>
     </row>
     <row r="11" spans="1:11" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="150"/>
+      <c r="A11" s="152"/>
       <c r="B11" s="100"/>
       <c r="C11" s="101"/>
       <c r="D11" s="101"/>
@@ -2577,19 +2647,19 @@
       <c r="F11" s="105"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="150"/>
+      <c r="A12" s="152"/>
       <c r="B12" s="98" t="s">
         <v>182</v>
       </c>
       <c r="C12" s="99">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="D12" s="99">
         <v>8430</v>
       </c>
       <c r="E12" s="101">
         <f t="shared" si="0"/>
-        <v>8351</v>
+        <v>8380</v>
       </c>
       <c r="F12" s="104"/>
     </row>
@@ -2601,8 +2671,7 @@
         <v>184</v>
       </c>
       <c r="C13" s="103">
-        <f>C12-C9</f>
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="D13" s="103">
         <f>D12-D9</f>
@@ -2610,17 +2679,17 @@
       </c>
       <c r="E13" s="122">
         <f>E12-E9</f>
-        <v>8351</v>
+        <v>8380</v>
       </c>
       <c r="F13" s="106"/>
       <c r="G13" s="112">
         <f>E13</f>
-        <v>8351</v>
+        <v>8380</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:11" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="151" t="s">
+      <c r="A15" s="153" t="s">
         <v>170</v>
       </c>
       <c r="B15" s="109" t="s">
@@ -2640,250 +2709,263 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="150"/>
+      <c r="A16" s="152"/>
       <c r="B16" s="98" t="s">
         <v>179</v>
       </c>
       <c r="C16" s="99">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="D16" s="99">
         <v>8430</v>
       </c>
       <c r="E16" s="123">
         <f t="shared" ref="E16:E33" si="1">IF(AND(C16&gt;0,D16&gt;0), D16-C16, 0)</f>
-        <v>8351</v>
+        <v>8380</v>
       </c>
       <c r="F16" s="104"/>
     </row>
-    <row r="17" spans="1:6" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="150"/>
-      <c r="B17" s="213" t="s">
+    <row r="17" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="152"/>
+      <c r="B17" s="149" t="s">
         <v>212</v>
       </c>
       <c r="C17" s="101">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="D17" s="101">
         <v>8430</v>
       </c>
       <c r="E17" s="124">
         <f t="shared" si="1"/>
-        <v>8351</v>
+        <v>8380</v>
       </c>
       <c r="F17" s="105"/>
-    </row>
-    <row r="18" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="150"/>
-      <c r="B18" s="213" t="s">
+      <c r="H17" s="112"/>
+    </row>
+    <row r="18" spans="1:8" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="152"/>
+      <c r="B18" s="149" t="s">
         <v>213</v>
       </c>
       <c r="C18" s="101">
-        <v>216</v>
+        <v>187</v>
       </c>
       <c r="D18" s="101">
         <v>8567</v>
       </c>
       <c r="E18" s="123">
         <f t="shared" si="1"/>
-        <v>8351</v>
+        <v>8380</v>
       </c>
       <c r="F18" s="105"/>
-    </row>
-    <row r="19" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="150"/>
-      <c r="B19" s="213" t="s">
+      <c r="H18" s="112"/>
+    </row>
+    <row r="19" spans="1:8" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="152"/>
+      <c r="B19" s="149" t="s">
         <v>215</v>
       </c>
       <c r="C19" s="101">
-        <v>254</v>
+        <v>225</v>
       </c>
       <c r="D19" s="101">
         <v>8605</v>
       </c>
       <c r="E19" s="123">
         <f t="shared" si="1"/>
-        <v>8351</v>
+        <v>8380</v>
       </c>
       <c r="F19" s="105"/>
-    </row>
-    <row r="20" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="150"/>
-      <c r="B20" s="213" t="s">
+      <c r="H19" s="112"/>
+    </row>
+    <row r="20" spans="1:8" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="152"/>
+      <c r="B20" s="149" t="s">
         <v>214</v>
       </c>
       <c r="C20" s="101">
-        <v>326</v>
+        <v>297</v>
       </c>
       <c r="D20" s="101">
         <v>8677</v>
       </c>
       <c r="E20" s="123">
         <f t="shared" si="1"/>
-        <v>8351</v>
+        <v>8380</v>
       </c>
       <c r="F20" s="105"/>
-    </row>
-    <row r="21" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="150"/>
-      <c r="B21" s="213" t="s">
+      <c r="H20" s="112"/>
+    </row>
+    <row r="21" spans="1:8" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="152"/>
+      <c r="B21" s="149" t="s">
         <v>216</v>
       </c>
       <c r="C21" s="101">
-        <v>388</v>
+        <v>359</v>
       </c>
       <c r="D21" s="101">
         <v>8739</v>
       </c>
       <c r="E21" s="123">
         <f t="shared" si="1"/>
-        <v>8351</v>
+        <v>8380</v>
       </c>
       <c r="F21" s="105"/>
-    </row>
-    <row r="22" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="150"/>
-      <c r="B22" s="213" t="s">
+      <c r="H21" s="112"/>
+    </row>
+    <row r="22" spans="1:8" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="152"/>
+      <c r="B22" s="149" t="s">
         <v>217</v>
       </c>
       <c r="C22" s="101">
-        <v>478</v>
+        <v>449</v>
       </c>
       <c r="D22" s="101">
         <v>8829</v>
       </c>
       <c r="E22" s="123">
         <f t="shared" si="1"/>
-        <v>8351</v>
+        <v>8380</v>
       </c>
       <c r="F22" s="105"/>
-    </row>
-    <row r="23" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="150"/>
-      <c r="B23" s="213" t="s">
+      <c r="H22" s="112"/>
+    </row>
+    <row r="23" spans="1:8" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="152"/>
+      <c r="B23" s="149" t="s">
         <v>218</v>
       </c>
       <c r="C23" s="101">
-        <v>556</v>
+        <v>527</v>
       </c>
       <c r="D23" s="101">
         <v>8907</v>
       </c>
       <c r="E23" s="123">
         <f t="shared" si="1"/>
-        <v>8351</v>
+        <v>8380</v>
       </c>
       <c r="F23" s="105"/>
-    </row>
-    <row r="24" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="150"/>
-      <c r="B24" s="213" t="s">
+      <c r="H23" s="112"/>
+    </row>
+    <row r="24" spans="1:8" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="152"/>
+      <c r="B24" s="149" t="s">
         <v>219</v>
       </c>
       <c r="C24" s="101">
-        <v>650</v>
+        <v>621</v>
       </c>
       <c r="D24" s="101">
         <v>9001</v>
       </c>
       <c r="E24" s="123">
         <f t="shared" si="1"/>
-        <v>8351</v>
+        <v>8380</v>
       </c>
       <c r="F24" s="105"/>
-    </row>
-    <row r="25" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="150"/>
-      <c r="B25" s="213" t="s">
+      <c r="H24" s="112"/>
+    </row>
+    <row r="25" spans="1:8" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="152"/>
+      <c r="B25" s="149" t="s">
         <v>220</v>
       </c>
       <c r="C25" s="101">
-        <v>906</v>
+        <v>877</v>
       </c>
       <c r="D25" s="101">
         <v>9257</v>
       </c>
       <c r="E25" s="123">
         <f t="shared" si="1"/>
-        <v>8351</v>
-      </c>
-      <c r="F25" s="214" t="s">
+        <v>8380</v>
+      </c>
+      <c r="F25" s="150" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="150"/>
-      <c r="B26" s="213" t="s">
+      <c r="H25" s="112"/>
+    </row>
+    <row r="26" spans="1:8" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="152"/>
+      <c r="B26" s="149" t="s">
         <v>222</v>
       </c>
       <c r="C26" s="101">
-        <v>1046</v>
+        <v>1017</v>
       </c>
       <c r="D26" s="101">
         <v>9397</v>
       </c>
       <c r="E26" s="123">
         <f t="shared" si="1"/>
-        <v>8351</v>
-      </c>
-      <c r="F26" s="214" t="s">
+        <v>8380</v>
+      </c>
+      <c r="F26" s="150" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="150"/>
-      <c r="B27" s="213" t="s">
+      <c r="H26" s="112"/>
+    </row>
+    <row r="27" spans="1:8" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="152"/>
+      <c r="B27" s="149" t="s">
         <v>223</v>
       </c>
       <c r="C27" s="101">
-        <v>1224</v>
+        <v>1195</v>
       </c>
       <c r="D27" s="101">
         <v>9575</v>
       </c>
       <c r="E27" s="123">
         <f t="shared" si="1"/>
-        <v>8351</v>
+        <v>8380</v>
       </c>
       <c r="F27" s="105"/>
-    </row>
-    <row r="28" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="150"/>
-      <c r="B28" s="213" t="s">
+      <c r="H27" s="112"/>
+    </row>
+    <row r="28" spans="1:8" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="152"/>
+      <c r="B28" s="149" t="s">
         <v>225</v>
       </c>
       <c r="C28" s="101">
-        <v>1314</v>
+        <v>1285</v>
       </c>
       <c r="D28" s="101">
         <v>9665</v>
       </c>
       <c r="E28" s="123">
         <f t="shared" si="1"/>
-        <v>8351</v>
+        <v>8380</v>
       </c>
       <c r="F28" s="105"/>
-    </row>
-    <row r="29" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="150"/>
-      <c r="B29" s="213" t="s">
+      <c r="H28" s="112"/>
+    </row>
+    <row r="29" spans="1:8" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="152"/>
+      <c r="B29" s="149" t="s">
         <v>226</v>
       </c>
       <c r="C29" s="101">
-        <v>1827</v>
+        <v>1798</v>
       </c>
       <c r="D29" s="101">
         <v>10178</v>
       </c>
       <c r="E29" s="123">
         <f t="shared" si="1"/>
-        <v>8351</v>
+        <v>8380</v>
       </c>
       <c r="F29" s="105"/>
-    </row>
-    <row r="30" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="150"/>
-      <c r="B30" s="213"/>
+      <c r="H29" s="112"/>
+    </row>
+    <row r="30" spans="1:8" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="152"/>
+      <c r="B30" s="149"/>
       <c r="C30" s="101"/>
       <c r="D30" s="101"/>
       <c r="E30" s="123">
@@ -2892,9 +2974,9 @@
       </c>
       <c r="F30" s="105"/>
     </row>
-    <row r="31" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="150"/>
-      <c r="B31" s="213"/>
+    <row r="31" spans="1:8" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="152"/>
+      <c r="B31" s="149"/>
       <c r="C31" s="101"/>
       <c r="D31" s="101"/>
       <c r="E31" s="123">
@@ -2903,37 +2985,37 @@
       </c>
       <c r="F31" s="105"/>
     </row>
-    <row r="32" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="150"/>
-      <c r="B32" s="213" t="s">
+    <row r="32" spans="1:8" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="152"/>
+      <c r="B32" s="149" t="s">
         <v>168</v>
       </c>
       <c r="C32" s="101">
-        <v>2039</v>
+        <v>2010</v>
       </c>
       <c r="D32" s="101">
         <v>10390</v>
       </c>
       <c r="E32" s="123">
         <f t="shared" si="1"/>
-        <v>8351</v>
+        <v>8380</v>
       </c>
       <c r="F32" s="105"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="150"/>
+      <c r="A33" s="152"/>
       <c r="B33" s="98" t="s">
         <v>182</v>
       </c>
       <c r="C33" s="99">
-        <v>2079</v>
+        <v>2050</v>
       </c>
       <c r="D33" s="99">
         <v>10430</v>
       </c>
       <c r="E33" s="125">
         <f t="shared" si="1"/>
-        <v>8351</v>
+        <v>8380</v>
       </c>
       <c r="F33" s="104"/>
     </row>
@@ -2964,7 +3046,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:7" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="149" t="s">
+      <c r="A36" s="151" t="s">
         <v>171</v>
       </c>
       <c r="B36" s="113" t="s">
@@ -2984,381 +3066,829 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="150"/>
+      <c r="A37" s="152"/>
       <c r="B37" s="98" t="s">
         <v>179</v>
       </c>
       <c r="C37" s="99">
-        <v>2079</v>
+        <v>2050</v>
       </c>
       <c r="D37" s="99">
         <v>10430</v>
       </c>
       <c r="E37" s="123">
-        <f t="shared" ref="E37:E50" si="2">IF(AND(C37&gt;0,D37&gt;0), D37-C37, 0)</f>
-        <v>8351</v>
+        <f t="shared" ref="E37:E76" si="2">IF(AND(C37&gt;0,D37&gt;0), D37-C37, 0)</f>
+        <v>8380</v>
       </c>
       <c r="F37" s="104"/>
     </row>
     <row r="38" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="150"/>
-      <c r="B38" s="213" t="s">
+      <c r="A38" s="152"/>
+      <c r="B38" s="149" t="s">
         <v>212</v>
       </c>
       <c r="C38" s="101">
-        <v>2079</v>
+        <v>2050</v>
       </c>
       <c r="D38" s="101">
         <v>10430</v>
       </c>
       <c r="E38" s="124">
         <f t="shared" si="2"/>
-        <v>8351</v>
+        <v>8380</v>
       </c>
       <c r="F38" s="105"/>
     </row>
     <row r="39" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="150"/>
-      <c r="B39" s="100"/>
-      <c r="C39" s="101"/>
-      <c r="D39" s="101"/>
+      <c r="A39" s="152"/>
+      <c r="B39" s="215" t="s">
+        <v>227</v>
+      </c>
+      <c r="C39" s="101">
+        <v>2183</v>
+      </c>
+      <c r="D39" s="101">
+        <v>10563</v>
+      </c>
       <c r="E39" s="123">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8380</v>
       </c>
       <c r="F39" s="105"/>
     </row>
     <row r="40" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="150"/>
-      <c r="B40" s="100"/>
-      <c r="C40" s="101"/>
-      <c r="D40" s="101"/>
+      <c r="A40" s="152"/>
+      <c r="B40" s="215" t="s">
+        <v>228</v>
+      </c>
+      <c r="C40" s="101">
+        <v>2447</v>
+      </c>
+      <c r="D40" s="101">
+        <v>10827</v>
+      </c>
       <c r="E40" s="123">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8380</v>
       </c>
       <c r="F40" s="105"/>
     </row>
     <row r="41" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="150"/>
-      <c r="B41" s="100"/>
-      <c r="C41" s="101"/>
-      <c r="D41" s="101"/>
+      <c r="A41" s="152"/>
+      <c r="B41" s="215" t="s">
+        <v>229</v>
+      </c>
+      <c r="C41" s="101">
+        <v>2599</v>
+      </c>
+      <c r="D41" s="101">
+        <v>10979</v>
+      </c>
       <c r="E41" s="123">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8380</v>
       </c>
       <c r="F41" s="105"/>
     </row>
     <row r="42" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="150"/>
-      <c r="B42" s="100"/>
-      <c r="C42" s="101"/>
-      <c r="D42" s="101"/>
+      <c r="A42" s="152"/>
+      <c r="B42" s="215" t="s">
+        <v>230</v>
+      </c>
+      <c r="C42" s="101">
+        <v>2727</v>
+      </c>
+      <c r="D42" s="101">
+        <v>11107</v>
+      </c>
       <c r="E42" s="123">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8380</v>
       </c>
       <c r="F42" s="105"/>
     </row>
     <row r="43" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="150"/>
-      <c r="B43" s="100"/>
-      <c r="C43" s="101"/>
-      <c r="D43" s="101"/>
+      <c r="A43" s="152"/>
+      <c r="B43" s="215" t="s">
+        <v>232</v>
+      </c>
+      <c r="C43" s="101">
+        <v>2903</v>
+      </c>
+      <c r="D43" s="101">
+        <v>11283</v>
+      </c>
       <c r="E43" s="123">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8380</v>
       </c>
       <c r="F43" s="105"/>
     </row>
     <row r="44" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="150"/>
-      <c r="B44" s="100"/>
-      <c r="C44" s="101"/>
-      <c r="D44" s="101"/>
+      <c r="A44" s="152"/>
+      <c r="B44" s="215" t="s">
+        <v>233</v>
+      </c>
+      <c r="C44" s="101">
+        <v>3121</v>
+      </c>
+      <c r="D44" s="101">
+        <v>11503</v>
+      </c>
       <c r="E44" s="123">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8382</v>
       </c>
       <c r="F44" s="105"/>
     </row>
     <row r="45" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="150"/>
-      <c r="B45" s="100"/>
-      <c r="C45" s="101"/>
-      <c r="D45" s="101"/>
+      <c r="A45" s="152"/>
+      <c r="B45" s="215" t="s">
+        <v>234</v>
+      </c>
+      <c r="C45" s="101">
+        <v>3229</v>
+      </c>
+      <c r="D45" s="101">
+        <v>11611</v>
+      </c>
       <c r="E45" s="123">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8382</v>
       </c>
       <c r="F45" s="105"/>
     </row>
     <row r="46" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="150"/>
-      <c r="B46" s="100"/>
-      <c r="C46" s="101"/>
-      <c r="D46" s="101"/>
+      <c r="A46" s="152"/>
+      <c r="B46" s="215" t="s">
+        <v>235</v>
+      </c>
+      <c r="C46" s="101">
+        <v>3307</v>
+      </c>
+      <c r="D46" s="101">
+        <v>11689</v>
+      </c>
       <c r="E46" s="123">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8382</v>
       </c>
       <c r="F46" s="105"/>
     </row>
     <row r="47" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="150"/>
-      <c r="B47" s="100"/>
-      <c r="C47" s="101"/>
-      <c r="D47" s="101"/>
+      <c r="A47" s="152"/>
+      <c r="B47" s="215" t="s">
+        <v>231</v>
+      </c>
+      <c r="C47" s="101">
+        <v>3409</v>
+      </c>
+      <c r="D47" s="101">
+        <v>11791</v>
+      </c>
       <c r="E47" s="123">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8382</v>
       </c>
       <c r="F47" s="105"/>
     </row>
     <row r="48" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="150"/>
-      <c r="B48" s="100"/>
-      <c r="C48" s="101"/>
-      <c r="D48" s="101"/>
+      <c r="A48" s="152"/>
+      <c r="B48" s="215" t="s">
+        <v>236</v>
+      </c>
+      <c r="C48" s="101">
+        <v>3477</v>
+      </c>
+      <c r="D48" s="101">
+        <v>11859</v>
+      </c>
       <c r="E48" s="123">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8382</v>
       </c>
       <c r="F48" s="105"/>
     </row>
-    <row r="49" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="150"/>
-      <c r="B49" s="100"/>
-      <c r="C49" s="101"/>
-      <c r="D49" s="101"/>
+    <row r="49" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="152"/>
+      <c r="B49" s="215" t="s">
+        <v>237</v>
+      </c>
+      <c r="C49" s="101">
+        <v>3609</v>
+      </c>
+      <c r="D49" s="101">
+        <v>11991</v>
+      </c>
       <c r="E49" s="123">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8382</v>
       </c>
       <c r="F49" s="105"/>
     </row>
-    <row r="50" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="150"/>
-      <c r="B50" s="98" t="s">
-        <v>182</v>
-      </c>
-      <c r="C50" s="99"/>
-      <c r="D50" s="99"/>
-      <c r="E50" s="125">
+    <row r="50" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="152"/>
+      <c r="B50" s="215" t="s">
+        <v>238</v>
+      </c>
+      <c r="C50" s="101">
+        <v>3611</v>
+      </c>
+      <c r="D50" s="101">
+        <v>11993</v>
+      </c>
+      <c r="E50" s="123">
+        <f t="shared" si="2"/>
+        <v>8382</v>
+      </c>
+      <c r="F50" s="105"/>
+    </row>
+    <row r="51" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="152"/>
+      <c r="B51" s="215" t="s">
+        <v>239</v>
+      </c>
+      <c r="C51" s="101">
+        <v>3727</v>
+      </c>
+      <c r="D51" s="101">
+        <v>12109</v>
+      </c>
+      <c r="E51" s="123">
+        <f t="shared" si="2"/>
+        <v>8382</v>
+      </c>
+      <c r="F51" s="105"/>
+    </row>
+    <row r="52" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="152"/>
+      <c r="B52" s="215" t="s">
+        <v>239</v>
+      </c>
+      <c r="C52" s="101">
+        <v>3728</v>
+      </c>
+      <c r="D52" s="101">
+        <v>12110</v>
+      </c>
+      <c r="E52" s="123">
+        <f t="shared" si="2"/>
+        <v>8382</v>
+      </c>
+      <c r="F52" s="105"/>
+    </row>
+    <row r="53" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="152"/>
+      <c r="B53" s="215" t="s">
+        <v>240</v>
+      </c>
+      <c r="C53" s="101">
+        <v>3743</v>
+      </c>
+      <c r="D53" s="101">
+        <v>12125</v>
+      </c>
+      <c r="E53" s="123">
+        <f t="shared" si="2"/>
+        <v>8382</v>
+      </c>
+      <c r="F53" s="105"/>
+    </row>
+    <row r="54" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="152"/>
+      <c r="B54" s="215" t="s">
+        <v>241</v>
+      </c>
+      <c r="C54" s="101">
+        <v>3857</v>
+      </c>
+      <c r="D54" s="101">
+        <v>12237</v>
+      </c>
+      <c r="E54" s="123">
+        <f t="shared" si="2"/>
+        <v>8380</v>
+      </c>
+      <c r="F54" s="105"/>
+    </row>
+    <row r="55" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="152"/>
+      <c r="B55" s="215" t="s">
+        <v>242</v>
+      </c>
+      <c r="C55" s="101">
+        <v>3979</v>
+      </c>
+      <c r="D55" s="101">
+        <v>12359</v>
+      </c>
+      <c r="E55" s="123">
+        <f t="shared" si="2"/>
+        <v>8380</v>
+      </c>
+      <c r="F55" s="105"/>
+    </row>
+    <row r="56" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="152"/>
+      <c r="B56" s="215" t="s">
+        <v>243</v>
+      </c>
+      <c r="C56" s="101">
+        <v>4043</v>
+      </c>
+      <c r="D56" s="101">
+        <v>12423</v>
+      </c>
+      <c r="E56" s="123">
+        <f t="shared" si="2"/>
+        <v>8380</v>
+      </c>
+      <c r="F56" s="105"/>
+    </row>
+    <row r="57" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="152"/>
+      <c r="B57" s="215" t="s">
+        <v>244</v>
+      </c>
+      <c r="C57" s="101">
+        <v>4153</v>
+      </c>
+      <c r="D57" s="101">
+        <v>12533</v>
+      </c>
+      <c r="E57" s="123">
+        <f t="shared" si="2"/>
+        <v>8380</v>
+      </c>
+      <c r="F57" s="105"/>
+    </row>
+    <row r="58" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="152"/>
+      <c r="B58" s="215" t="s">
+        <v>245</v>
+      </c>
+      <c r="C58" s="101">
+        <v>4187</v>
+      </c>
+      <c r="D58" s="101">
+        <v>12567</v>
+      </c>
+      <c r="E58" s="123">
+        <f t="shared" si="2"/>
+        <v>8380</v>
+      </c>
+      <c r="F58" s="105"/>
+    </row>
+    <row r="59" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="152"/>
+      <c r="B59" s="215" t="s">
+        <v>246</v>
+      </c>
+      <c r="C59" s="101">
+        <v>4190</v>
+      </c>
+      <c r="D59" s="101">
+        <v>12570</v>
+      </c>
+      <c r="E59" s="123">
+        <f t="shared" si="2"/>
+        <v>8380</v>
+      </c>
+      <c r="F59" s="105"/>
+    </row>
+    <row r="60" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="152"/>
+      <c r="B60" s="215"/>
+      <c r="C60" s="101">
+        <v>4218</v>
+      </c>
+      <c r="D60" s="101">
+        <v>12598</v>
+      </c>
+      <c r="E60" s="123">
+        <f t="shared" si="2"/>
+        <v>8380</v>
+      </c>
+      <c r="F60" s="105"/>
+    </row>
+    <row r="61" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="152"/>
+      <c r="B61" s="215"/>
+      <c r="C61" s="101">
+        <v>4225</v>
+      </c>
+      <c r="D61" s="101">
+        <v>12605</v>
+      </c>
+      <c r="E61" s="123">
+        <f t="shared" si="2"/>
+        <v>8380</v>
+      </c>
+      <c r="F61" s="105"/>
+    </row>
+    <row r="62" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="152"/>
+      <c r="B62" s="215"/>
+      <c r="C62" s="101">
+        <v>4230</v>
+      </c>
+      <c r="D62" s="101">
+        <v>12610</v>
+      </c>
+      <c r="E62" s="123">
+        <f t="shared" si="2"/>
+        <v>8380</v>
+      </c>
+      <c r="F62" s="105"/>
+    </row>
+    <row r="63" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="152"/>
+      <c r="B63" s="215"/>
+      <c r="C63" s="101">
+        <v>4244</v>
+      </c>
+      <c r="D63" s="101">
+        <v>12624</v>
+      </c>
+      <c r="E63" s="123">
+        <f t="shared" si="2"/>
+        <v>8380</v>
+      </c>
+      <c r="F63" s="105"/>
+    </row>
+    <row r="64" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="152"/>
+      <c r="B64" s="215"/>
+      <c r="C64" s="101">
+        <v>4250</v>
+      </c>
+      <c r="D64" s="101">
+        <v>12630</v>
+      </c>
+      <c r="E64" s="123">
+        <f t="shared" si="2"/>
+        <v>8380</v>
+      </c>
+      <c r="F64" s="105"/>
+    </row>
+    <row r="65" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="152"/>
+      <c r="B65" s="215"/>
+      <c r="C65" s="101">
+        <v>4258</v>
+      </c>
+      <c r="D65" s="101">
+        <v>12638</v>
+      </c>
+      <c r="E65" s="123">
+        <f t="shared" si="2"/>
+        <v>8380</v>
+      </c>
+      <c r="F65" s="105"/>
+    </row>
+    <row r="66" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="152"/>
+      <c r="B66" s="215"/>
+      <c r="C66" s="101">
+        <v>4260</v>
+      </c>
+      <c r="D66" s="101">
+        <v>12640</v>
+      </c>
+      <c r="E66" s="123">
+        <f t="shared" si="2"/>
+        <v>8380</v>
+      </c>
+      <c r="F66" s="105"/>
+    </row>
+    <row r="67" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="152"/>
+      <c r="B67" s="215"/>
+      <c r="C67" s="101">
+        <v>4282</v>
+      </c>
+      <c r="D67" s="101">
+        <v>12662</v>
+      </c>
+      <c r="E67" s="123">
+        <f t="shared" si="2"/>
+        <v>8380</v>
+      </c>
+      <c r="F67" s="105"/>
+    </row>
+    <row r="68" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="152"/>
+      <c r="B68" s="215"/>
+      <c r="C68" s="101"/>
+      <c r="D68" s="101"/>
+      <c r="E68" s="123">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F50" s="104"/>
-    </row>
-    <row r="51" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="116">
-        <v>6</v>
-      </c>
-      <c r="B51" s="102" t="s">
+      <c r="F68" s="105"/>
+    </row>
+    <row r="69" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="152"/>
+      <c r="B69" s="215"/>
+      <c r="C69" s="101"/>
+      <c r="D69" s="101"/>
+      <c r="E69" s="123">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F69" s="105"/>
+    </row>
+    <row r="70" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="152"/>
+      <c r="B70" s="215"/>
+      <c r="C70" s="101"/>
+      <c r="D70" s="101"/>
+      <c r="E70" s="123">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F70" s="105"/>
+    </row>
+    <row r="71" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="152"/>
+      <c r="B71" s="215"/>
+      <c r="C71" s="101"/>
+      <c r="D71" s="101"/>
+      <c r="E71" s="123">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F71" s="105"/>
+    </row>
+    <row r="72" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="152"/>
+      <c r="B72" s="215"/>
+      <c r="C72" s="101"/>
+      <c r="D72" s="101"/>
+      <c r="E72" s="123">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F72" s="105"/>
+    </row>
+    <row r="73" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="152"/>
+      <c r="B73" s="215"/>
+      <c r="C73" s="101"/>
+      <c r="D73" s="101"/>
+      <c r="E73" s="123">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F73" s="105"/>
+    </row>
+    <row r="74" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="152"/>
+      <c r="B74" s="100"/>
+      <c r="C74" s="101"/>
+      <c r="D74" s="101"/>
+      <c r="E74" s="123">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F74" s="105"/>
+    </row>
+    <row r="75" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="152"/>
+      <c r="B75" s="100"/>
+      <c r="C75" s="101"/>
+      <c r="D75" s="101"/>
+      <c r="E75" s="123">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F75" s="105"/>
+    </row>
+    <row r="76" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="152"/>
+      <c r="B76" s="98" t="s">
+        <v>182</v>
+      </c>
+      <c r="C76" s="99">
+        <v>4298</v>
+      </c>
+      <c r="D76" s="99">
+        <v>12678</v>
+      </c>
+      <c r="E76" s="125">
+        <f t="shared" si="2"/>
+        <v>8380</v>
+      </c>
+      <c r="F76" s="104"/>
+    </row>
+    <row r="77" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="116">
+        <v>6</v>
+      </c>
+      <c r="B77" s="102" t="s">
         <v>175</v>
       </c>
-      <c r="C51" s="103">
-        <f>C50-C37</f>
-        <v>-2079</v>
-      </c>
-      <c r="D51" s="103">
-        <f>D50-D37</f>
-        <v>-10430</v>
-      </c>
-      <c r="E51" s="126">
-        <f>E50-E37</f>
-        <v>-8351</v>
-      </c>
-      <c r="F51" s="107"/>
-      <c r="G51" s="112">
-        <f>E51</f>
-        <v>-8351</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="151" t="s">
+      <c r="C77" s="103">
+        <f>C76-C37</f>
+        <v>2248</v>
+      </c>
+      <c r="D77" s="103">
+        <f>D76-D37</f>
+        <v>2248</v>
+      </c>
+      <c r="E77" s="126">
+        <f>E76-E37</f>
+        <v>0</v>
+      </c>
+      <c r="F77" s="107"/>
+      <c r="G77" s="112">
+        <f>E77</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="153" t="s">
         <v>169</v>
       </c>
-      <c r="B53" s="109" t="s">
+      <c r="B79" s="109" t="s">
         <v>177</v>
       </c>
-      <c r="C53" s="110" t="s">
+      <c r="C79" s="110" t="s">
         <v>42</v>
       </c>
-      <c r="D53" s="110" t="s">
+      <c r="D79" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="E53" s="110" t="s">
+      <c r="E79" s="110" t="s">
         <v>43</v>
       </c>
-      <c r="F53" s="111" t="s">
+      <c r="F79" s="111" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="150"/>
-      <c r="B54" s="98" t="s">
+    <row r="80" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="152"/>
+      <c r="B80" s="98" t="s">
         <v>179</v>
       </c>
-      <c r="C54" s="99"/>
-      <c r="D54" s="99"/>
-      <c r="E54" s="123">
-        <f t="shared" ref="E54:E67" si="3">IF(AND(C54&gt;0,D54&gt;0), D54-C54, 0)</f>
+      <c r="C80" s="99"/>
+      <c r="D80" s="99"/>
+      <c r="E80" s="123">
+        <f t="shared" ref="E80:E93" si="3">IF(AND(C80&gt;0,D80&gt;0), D80-C80, 0)</f>
         <v>0</v>
       </c>
-      <c r="F54" s="104"/>
-    </row>
-    <row r="55" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="150"/>
-      <c r="B55" s="100"/>
-      <c r="C55" s="101"/>
-      <c r="D55" s="101"/>
-      <c r="E55" s="124">
+      <c r="F80" s="104"/>
+    </row>
+    <row r="81" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="152"/>
+      <c r="B81" s="100"/>
+      <c r="C81" s="101"/>
+      <c r="D81" s="101"/>
+      <c r="E81" s="124">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F55" s="105"/>
-    </row>
-    <row r="56" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="150"/>
-      <c r="B56" s="100"/>
-      <c r="C56" s="101"/>
-      <c r="D56" s="101"/>
-      <c r="E56" s="123">
+      <c r="F81" s="105"/>
+    </row>
+    <row r="82" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="152"/>
+      <c r="B82" s="100"/>
+      <c r="C82" s="101"/>
+      <c r="D82" s="101"/>
+      <c r="E82" s="123">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F56" s="105"/>
-    </row>
-    <row r="57" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="150"/>
-      <c r="B57" s="100"/>
-      <c r="C57" s="101"/>
-      <c r="D57" s="101"/>
-      <c r="E57" s="123">
+      <c r="F82" s="105"/>
+    </row>
+    <row r="83" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="152"/>
+      <c r="B83" s="100"/>
+      <c r="C83" s="101"/>
+      <c r="D83" s="101"/>
+      <c r="E83" s="123">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F57" s="105"/>
-    </row>
-    <row r="58" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="150"/>
-      <c r="B58" s="100"/>
-      <c r="C58" s="101"/>
-      <c r="D58" s="101"/>
-      <c r="E58" s="123">
+      <c r="F83" s="105"/>
+    </row>
+    <row r="84" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="152"/>
+      <c r="B84" s="100"/>
+      <c r="C84" s="101"/>
+      <c r="D84" s="101"/>
+      <c r="E84" s="123">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F58" s="105"/>
-    </row>
-    <row r="59" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="150"/>
-      <c r="B59" s="100"/>
-      <c r="C59" s="101"/>
-      <c r="D59" s="101"/>
-      <c r="E59" s="123">
+      <c r="F84" s="105"/>
+    </row>
+    <row r="85" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="152"/>
+      <c r="B85" s="100"/>
+      <c r="C85" s="101"/>
+      <c r="D85" s="101"/>
+      <c r="E85" s="123">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F59" s="105"/>
-    </row>
-    <row r="60" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="150"/>
-      <c r="B60" s="100"/>
-      <c r="C60" s="101"/>
-      <c r="D60" s="101"/>
-      <c r="E60" s="123">
+      <c r="F85" s="105"/>
+    </row>
+    <row r="86" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="152"/>
+      <c r="B86" s="100"/>
+      <c r="C86" s="101"/>
+      <c r="D86" s="101"/>
+      <c r="E86" s="123">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F60" s="105"/>
-    </row>
-    <row r="61" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="150"/>
-      <c r="B61" s="100"/>
-      <c r="C61" s="101"/>
-      <c r="D61" s="101"/>
-      <c r="E61" s="123">
+      <c r="F86" s="105"/>
+    </row>
+    <row r="87" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="152"/>
+      <c r="B87" s="100"/>
+      <c r="C87" s="101"/>
+      <c r="D87" s="101"/>
+      <c r="E87" s="123">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F61" s="105"/>
-    </row>
-    <row r="62" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="150"/>
-      <c r="B62" s="100"/>
-      <c r="C62" s="101"/>
-      <c r="D62" s="101"/>
-      <c r="E62" s="123">
+      <c r="F87" s="105"/>
+    </row>
+    <row r="88" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="152"/>
+      <c r="B88" s="100"/>
+      <c r="C88" s="101"/>
+      <c r="D88" s="101"/>
+      <c r="E88" s="123">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F62" s="105"/>
-    </row>
-    <row r="63" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="150"/>
-      <c r="B63" s="100"/>
-      <c r="C63" s="101"/>
-      <c r="D63" s="101"/>
-      <c r="E63" s="123">
+      <c r="F88" s="105"/>
+    </row>
+    <row r="89" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="152"/>
+      <c r="B89" s="100"/>
+      <c r="C89" s="101"/>
+      <c r="D89" s="101"/>
+      <c r="E89" s="123">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F63" s="105"/>
-    </row>
-    <row r="64" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="150"/>
-      <c r="B64" s="100"/>
-      <c r="C64" s="101"/>
-      <c r="D64" s="101"/>
-      <c r="E64" s="123">
+      <c r="F89" s="105"/>
+    </row>
+    <row r="90" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="152"/>
+      <c r="B90" s="100"/>
+      <c r="C90" s="101"/>
+      <c r="D90" s="101"/>
+      <c r="E90" s="123">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F64" s="105"/>
-    </row>
-    <row r="65" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="150"/>
-      <c r="B65" s="100"/>
-      <c r="C65" s="101"/>
-      <c r="D65" s="101"/>
-      <c r="E65" s="123">
+      <c r="F90" s="105"/>
+    </row>
+    <row r="91" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="152"/>
+      <c r="B91" s="100"/>
+      <c r="C91" s="101"/>
+      <c r="D91" s="101"/>
+      <c r="E91" s="123">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F65" s="105"/>
-    </row>
-    <row r="66" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="150"/>
-      <c r="B66" s="100"/>
-      <c r="C66" s="101"/>
-      <c r="D66" s="101"/>
-      <c r="E66" s="123">
+      <c r="F91" s="105"/>
+    </row>
+    <row r="92" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="152"/>
+      <c r="B92" s="100"/>
+      <c r="C92" s="101"/>
+      <c r="D92" s="101"/>
+      <c r="E92" s="123">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F66" s="105"/>
-    </row>
-    <row r="67" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="150"/>
-      <c r="B67" s="98" t="s">
+      <c r="F92" s="105"/>
+    </row>
+    <row r="93" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="152"/>
+      <c r="B93" s="98" t="s">
         <v>182</v>
       </c>
-      <c r="C67" s="99"/>
-      <c r="D67" s="99"/>
-      <c r="E67" s="125">
+      <c r="C93" s="99"/>
+      <c r="D93" s="99"/>
+      <c r="E93" s="125">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F67" s="104"/>
-    </row>
-    <row r="68" spans="1:6" collapsed="1" x14ac:dyDescent="0.2"/>
+      <c r="F93" s="104"/>
+    </row>
+    <row r="94" spans="1:6" collapsed="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A36:A50"/>
-    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="A36:A76"/>
+    <mergeCell ref="A79:A93"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="A1:B1"/>
@@ -3396,13 +3926,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="158"/>
-      <c r="C1" s="158"/>
-      <c r="D1" s="158"/>
-      <c r="E1" s="158"/>
+      <c r="B1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="160"/>
+      <c r="E1" s="160"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -3432,18 +3962,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="159"/>
-      <c r="D3" s="160"/>
-      <c r="E3" s="160"/>
+      <c r="C3" s="161"/>
+      <c r="D3" s="162"/>
+      <c r="E3" s="162"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="161"/>
-      <c r="D4" s="162"/>
-      <c r="E4" s="162"/>
+      <c r="C4" s="163"/>
+      <c r="D4" s="164"/>
+      <c r="E4" s="164"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -3595,9 +4125,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="163"/>
-      <c r="D21" s="164"/>
-      <c r="E21" s="164"/>
+      <c r="C21" s="165"/>
+      <c r="D21" s="166"/>
+      <c r="E21" s="166"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A22" s="47">
@@ -3748,9 +4278,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="161"/>
-      <c r="D38" s="162"/>
-      <c r="E38" s="162"/>
+      <c r="C38" s="163"/>
+      <c r="D38" s="164"/>
+      <c r="E38" s="164"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A39" s="47">
@@ -3901,9 +4431,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="161"/>
-      <c r="D55" s="162"/>
-      <c r="E55" s="162"/>
+      <c r="C55" s="163"/>
+      <c r="D55" s="164"/>
+      <c r="E55" s="164"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A56" s="47">
@@ -4054,9 +4584,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="161"/>
-      <c r="D72" s="162"/>
-      <c r="E72" s="162"/>
+      <c r="C72" s="163"/>
+      <c r="D72" s="164"/>
+      <c r="E72" s="164"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A73" s="47">
@@ -4207,9 +4737,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="161"/>
-      <c r="D89" s="162"/>
-      <c r="E89" s="162"/>
+      <c r="C89" s="163"/>
+      <c r="D89" s="164"/>
+      <c r="E89" s="164"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A90" s="47">
@@ -4360,9 +4890,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="161"/>
-      <c r="D106" s="162"/>
-      <c r="E106" s="162"/>
+      <c r="C106" s="163"/>
+      <c r="D106" s="164"/>
+      <c r="E106" s="164"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A107" s="47">
@@ -4513,9 +5043,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="161"/>
-      <c r="D123" s="162"/>
-      <c r="E123" s="162"/>
+      <c r="C123" s="163"/>
+      <c r="D123" s="164"/>
+      <c r="E123" s="164"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A124" s="47">
@@ -4666,9 +5196,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="161"/>
-      <c r="D140" s="162"/>
-      <c r="E140" s="162"/>
+      <c r="C140" s="163"/>
+      <c r="D140" s="164"/>
+      <c r="E140" s="164"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A141" s="47">
@@ -4819,9 +5349,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="161"/>
-      <c r="D157" s="162"/>
-      <c r="E157" s="162"/>
+      <c r="C157" s="163"/>
+      <c r="D157" s="164"/>
+      <c r="E157" s="164"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A158" s="47">
@@ -4972,9 +5502,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="161"/>
-      <c r="D174" s="162"/>
-      <c r="E174" s="162"/>
+      <c r="C174" s="163"/>
+      <c r="D174" s="164"/>
+      <c r="E174" s="164"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A175" s="47">
@@ -5125,9 +5655,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="161"/>
-      <c r="D191" s="162"/>
-      <c r="E191" s="162"/>
+      <c r="C191" s="163"/>
+      <c r="D191" s="164"/>
+      <c r="E191" s="164"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A192" s="47">
@@ -5278,9 +5808,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="161"/>
-      <c r="D208" s="162"/>
-      <c r="E208" s="162"/>
+      <c r="C208" s="163"/>
+      <c r="D208" s="164"/>
+      <c r="E208" s="164"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A209" s="47">
@@ -5431,9 +5961,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="161"/>
-      <c r="D225" s="162"/>
-      <c r="E225" s="162"/>
+      <c r="C225" s="163"/>
+      <c r="D225" s="164"/>
+      <c r="E225" s="164"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A226" s="47">
@@ -5584,9 +6114,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="161"/>
-      <c r="D242" s="162"/>
-      <c r="E242" s="162"/>
+      <c r="C242" s="163"/>
+      <c r="D242" s="164"/>
+      <c r="E242" s="164"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A243" s="47">
@@ -5737,9 +6267,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="161"/>
-      <c r="D259" s="162"/>
-      <c r="E259" s="162"/>
+      <c r="C259" s="163"/>
+      <c r="D259" s="164"/>
+      <c r="E259" s="164"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A260" s="47">
@@ -5890,18 +6420,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="165"/>
-      <c r="D276" s="166"/>
-      <c r="E276" s="166"/>
+      <c r="C276" s="167"/>
+      <c r="D276" s="168"/>
+      <c r="E276" s="168"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="161"/>
-      <c r="D277" s="162"/>
-      <c r="E277" s="162"/>
+      <c r="C277" s="163"/>
+      <c r="D277" s="164"/>
+      <c r="E277" s="164"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A278" s="52">
@@ -6052,9 +6582,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="163"/>
-      <c r="D294" s="164"/>
-      <c r="E294" s="164"/>
+      <c r="C294" s="165"/>
+      <c r="D294" s="166"/>
+      <c r="E294" s="166"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A295" s="52">
@@ -6205,9 +6735,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="161"/>
-      <c r="D311" s="162"/>
-      <c r="E311" s="162"/>
+      <c r="C311" s="163"/>
+      <c r="D311" s="164"/>
+      <c r="E311" s="164"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A312" s="52">
@@ -6358,9 +6888,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="161"/>
-      <c r="D328" s="162"/>
-      <c r="E328" s="162"/>
+      <c r="C328" s="163"/>
+      <c r="D328" s="164"/>
+      <c r="E328" s="164"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A329" s="52">
@@ -6511,9 +7041,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="161"/>
-      <c r="D345" s="162"/>
-      <c r="E345" s="162"/>
+      <c r="C345" s="163"/>
+      <c r="D345" s="164"/>
+      <c r="E345" s="164"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A346" s="52">
@@ -6664,9 +7194,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="161"/>
-      <c r="D362" s="162"/>
-      <c r="E362" s="162"/>
+      <c r="C362" s="163"/>
+      <c r="D362" s="164"/>
+      <c r="E362" s="164"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A363" s="52">
@@ -6817,9 +7347,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="161"/>
-      <c r="D379" s="162"/>
-      <c r="E379" s="162"/>
+      <c r="C379" s="163"/>
+      <c r="D379" s="164"/>
+      <c r="E379" s="164"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A380" s="52">
@@ -6970,9 +7500,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="161"/>
-      <c r="D396" s="162"/>
-      <c r="E396" s="162"/>
+      <c r="C396" s="163"/>
+      <c r="D396" s="164"/>
+      <c r="E396" s="164"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A397" s="52">
@@ -7123,9 +7653,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="161"/>
-      <c r="D413" s="162"/>
-      <c r="E413" s="162"/>
+      <c r="C413" s="163"/>
+      <c r="D413" s="164"/>
+      <c r="E413" s="164"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A414" s="52">
@@ -7276,9 +7806,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="161"/>
-      <c r="D430" s="162"/>
-      <c r="E430" s="162"/>
+      <c r="C430" s="163"/>
+      <c r="D430" s="164"/>
+      <c r="E430" s="164"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A431" s="52">
@@ -7429,9 +7959,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="161"/>
-      <c r="D447" s="162"/>
-      <c r="E447" s="162"/>
+      <c r="C447" s="163"/>
+      <c r="D447" s="164"/>
+      <c r="E447" s="164"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A448" s="52">
@@ -7582,9 +8112,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="161"/>
-      <c r="D464" s="162"/>
-      <c r="E464" s="162"/>
+      <c r="C464" s="163"/>
+      <c r="D464" s="164"/>
+      <c r="E464" s="164"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A465" s="52">
@@ -7735,9 +8265,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="161"/>
-      <c r="D481" s="162"/>
-      <c r="E481" s="162"/>
+      <c r="C481" s="163"/>
+      <c r="D481" s="164"/>
+      <c r="E481" s="164"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A482" s="52">
@@ -7888,9 +8418,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="161"/>
-      <c r="D498" s="162"/>
-      <c r="E498" s="162"/>
+      <c r="C498" s="163"/>
+      <c r="D498" s="164"/>
+      <c r="E498" s="164"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A499" s="52">
@@ -8041,9 +8571,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="161"/>
-      <c r="D515" s="162"/>
-      <c r="E515" s="162"/>
+      <c r="C515" s="163"/>
+      <c r="D515" s="164"/>
+      <c r="E515" s="164"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A516" s="52">
@@ -8194,9 +8724,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="161"/>
-      <c r="D532" s="162"/>
-      <c r="E532" s="162"/>
+      <c r="C532" s="163"/>
+      <c r="D532" s="164"/>
+      <c r="E532" s="164"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A533" s="55">
@@ -8347,18 +8877,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="167"/>
-      <c r="D549" s="168"/>
-      <c r="E549" s="168"/>
+      <c r="C549" s="169"/>
+      <c r="D549" s="170"/>
+      <c r="E549" s="170"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="161"/>
-      <c r="D550" s="162"/>
-      <c r="E550" s="162"/>
+      <c r="C550" s="163"/>
+      <c r="D550" s="164"/>
+      <c r="E550" s="164"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A551" s="59">
@@ -8509,9 +9039,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="163"/>
-      <c r="D567" s="164"/>
-      <c r="E567" s="164"/>
+      <c r="C567" s="165"/>
+      <c r="D567" s="166"/>
+      <c r="E567" s="166"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A568" s="59">
@@ -8662,9 +9192,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="161"/>
-      <c r="D584" s="162"/>
-      <c r="E584" s="162"/>
+      <c r="C584" s="163"/>
+      <c r="D584" s="164"/>
+      <c r="E584" s="164"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A585" s="59">
@@ -8815,9 +9345,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="161"/>
-      <c r="D601" s="162"/>
-      <c r="E601" s="162"/>
+      <c r="C601" s="163"/>
+      <c r="D601" s="164"/>
+      <c r="E601" s="164"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A602" s="59">
@@ -8968,9 +9498,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="161"/>
-      <c r="D618" s="162"/>
-      <c r="E618" s="162"/>
+      <c r="C618" s="163"/>
+      <c r="D618" s="164"/>
+      <c r="E618" s="164"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A619" s="59">
@@ -9121,9 +9651,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="161"/>
-      <c r="D635" s="162"/>
-      <c r="E635" s="162"/>
+      <c r="C635" s="163"/>
+      <c r="D635" s="164"/>
+      <c r="E635" s="164"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A636" s="59">
@@ -9274,9 +9804,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="161"/>
-      <c r="D652" s="162"/>
-      <c r="E652" s="162"/>
+      <c r="C652" s="163"/>
+      <c r="D652" s="164"/>
+      <c r="E652" s="164"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A653" s="59">
@@ -9427,9 +9957,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="161"/>
-      <c r="D669" s="162"/>
-      <c r="E669" s="162"/>
+      <c r="C669" s="163"/>
+      <c r="D669" s="164"/>
+      <c r="E669" s="164"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A670" s="59">
@@ -9580,9 +10110,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="161"/>
-      <c r="D686" s="162"/>
-      <c r="E686" s="162"/>
+      <c r="C686" s="163"/>
+      <c r="D686" s="164"/>
+      <c r="E686" s="164"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A687" s="59">
@@ -9733,9 +10263,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="161"/>
-      <c r="D703" s="162"/>
-      <c r="E703" s="162"/>
+      <c r="C703" s="163"/>
+      <c r="D703" s="164"/>
+      <c r="E703" s="164"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A704" s="59">
@@ -9886,9 +10416,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="161"/>
-      <c r="D720" s="162"/>
-      <c r="E720" s="162"/>
+      <c r="C720" s="163"/>
+      <c r="D720" s="164"/>
+      <c r="E720" s="164"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A721" s="59">
@@ -10039,9 +10569,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="161"/>
-      <c r="D737" s="162"/>
-      <c r="E737" s="162"/>
+      <c r="C737" s="163"/>
+      <c r="D737" s="164"/>
+      <c r="E737" s="164"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A738" s="59">
@@ -10192,9 +10722,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="161"/>
-      <c r="D754" s="162"/>
-      <c r="E754" s="162"/>
+      <c r="C754" s="163"/>
+      <c r="D754" s="164"/>
+      <c r="E754" s="164"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A755" s="59">
@@ -10345,9 +10875,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="161"/>
-      <c r="D771" s="162"/>
-      <c r="E771" s="162"/>
+      <c r="C771" s="163"/>
+      <c r="D771" s="164"/>
+      <c r="E771" s="164"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A772" s="59">
@@ -10498,9 +11028,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="161"/>
-      <c r="D788" s="162"/>
-      <c r="E788" s="162"/>
+      <c r="C788" s="163"/>
+      <c r="D788" s="164"/>
+      <c r="E788" s="164"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A789" s="59">
@@ -10651,9 +11181,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="161"/>
-      <c r="D805" s="162"/>
-      <c r="E805" s="162"/>
+      <c r="C805" s="163"/>
+      <c r="D805" s="164"/>
+      <c r="E805" s="164"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A806" s="59">
@@ -10804,18 +11334,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="169"/>
-      <c r="D822" s="170"/>
-      <c r="E822" s="170"/>
+      <c r="C822" s="171"/>
+      <c r="D822" s="172"/>
+      <c r="E822" s="172"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="161"/>
-      <c r="D823" s="162"/>
-      <c r="E823" s="162"/>
+      <c r="C823" s="163"/>
+      <c r="D823" s="164"/>
+      <c r="E823" s="164"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A824" s="64">
@@ -10966,9 +11496,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="163"/>
-      <c r="D840" s="164"/>
-      <c r="E840" s="164"/>
+      <c r="C840" s="165"/>
+      <c r="D840" s="166"/>
+      <c r="E840" s="166"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A841" s="64">
@@ -11119,9 +11649,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="161"/>
-      <c r="D857" s="162"/>
-      <c r="E857" s="162"/>
+      <c r="C857" s="163"/>
+      <c r="D857" s="164"/>
+      <c r="E857" s="164"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A858" s="64">
@@ -11272,9 +11802,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="161"/>
-      <c r="D874" s="162"/>
-      <c r="E874" s="162"/>
+      <c r="C874" s="163"/>
+      <c r="D874" s="164"/>
+      <c r="E874" s="164"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A875" s="64">
@@ -11425,9 +11955,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="161"/>
-      <c r="D891" s="162"/>
-      <c r="E891" s="162"/>
+      <c r="C891" s="163"/>
+      <c r="D891" s="164"/>
+      <c r="E891" s="164"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A892" s="64">
@@ -11578,9 +12108,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="161"/>
-      <c r="D908" s="162"/>
-      <c r="E908" s="162"/>
+      <c r="C908" s="163"/>
+      <c r="D908" s="164"/>
+      <c r="E908" s="164"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A909" s="64">
@@ -11731,9 +12261,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="161"/>
-      <c r="D925" s="162"/>
-      <c r="E925" s="162"/>
+      <c r="C925" s="163"/>
+      <c r="D925" s="164"/>
+      <c r="E925" s="164"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A926" s="64">
@@ -11884,9 +12414,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="161"/>
-      <c r="D942" s="162"/>
-      <c r="E942" s="162"/>
+      <c r="C942" s="163"/>
+      <c r="D942" s="164"/>
+      <c r="E942" s="164"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A943" s="64">
@@ -12037,9 +12567,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="161"/>
-      <c r="D959" s="162"/>
-      <c r="E959" s="162"/>
+      <c r="C959" s="163"/>
+      <c r="D959" s="164"/>
+      <c r="E959" s="164"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A960" s="64">
@@ -12190,9 +12720,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="161"/>
-      <c r="D976" s="162"/>
-      <c r="E976" s="162"/>
+      <c r="C976" s="163"/>
+      <c r="D976" s="164"/>
+      <c r="E976" s="164"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A977" s="64">
@@ -12343,9 +12873,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="161"/>
-      <c r="D993" s="162"/>
-      <c r="E993" s="162"/>
+      <c r="C993" s="163"/>
+      <c r="D993" s="164"/>
+      <c r="E993" s="164"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A994" s="64">
@@ -12496,9 +13026,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="161"/>
-      <c r="D1010" s="162"/>
-      <c r="E1010" s="162"/>
+      <c r="C1010" s="163"/>
+      <c r="D1010" s="164"/>
+      <c r="E1010" s="164"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1011" s="64">
@@ -12649,9 +13179,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="161"/>
-      <c r="D1027" s="162"/>
-      <c r="E1027" s="162"/>
+      <c r="C1027" s="163"/>
+      <c r="D1027" s="164"/>
+      <c r="E1027" s="164"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1028" s="64">
@@ -12802,9 +13332,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="161"/>
-      <c r="D1044" s="162"/>
-      <c r="E1044" s="162"/>
+      <c r="C1044" s="163"/>
+      <c r="D1044" s="164"/>
+      <c r="E1044" s="164"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1045" s="64">
@@ -12955,9 +13485,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="161"/>
-      <c r="D1061" s="162"/>
-      <c r="E1061" s="162"/>
+      <c r="C1061" s="163"/>
+      <c r="D1061" s="164"/>
+      <c r="E1061" s="164"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1062" s="64">
@@ -13108,9 +13638,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="161"/>
-      <c r="D1078" s="162"/>
-      <c r="E1078" s="162"/>
+      <c r="C1078" s="163"/>
+      <c r="D1078" s="164"/>
+      <c r="E1078" s="164"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1079" s="64">
@@ -13261,18 +13791,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="171"/>
-      <c r="D1095" s="172"/>
-      <c r="E1095" s="172"/>
+      <c r="C1095" s="173"/>
+      <c r="D1095" s="174"/>
+      <c r="E1095" s="174"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="161"/>
-      <c r="D1096" s="162"/>
-      <c r="E1096" s="162"/>
+      <c r="C1096" s="163"/>
+      <c r="D1096" s="164"/>
+      <c r="E1096" s="164"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1097" s="69">
@@ -13423,9 +13953,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="163"/>
-      <c r="D1113" s="164"/>
-      <c r="E1113" s="164"/>
+      <c r="C1113" s="165"/>
+      <c r="D1113" s="166"/>
+      <c r="E1113" s="166"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1114" s="69">
@@ -13576,9 +14106,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="161"/>
-      <c r="D1130" s="162"/>
-      <c r="E1130" s="162"/>
+      <c r="C1130" s="163"/>
+      <c r="D1130" s="164"/>
+      <c r="E1130" s="164"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1131" s="69">
@@ -13729,9 +14259,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="161"/>
-      <c r="D1147" s="162"/>
-      <c r="E1147" s="162"/>
+      <c r="C1147" s="163"/>
+      <c r="D1147" s="164"/>
+      <c r="E1147" s="164"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1148" s="69">
@@ -13882,9 +14412,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="161"/>
-      <c r="D1164" s="162"/>
-      <c r="E1164" s="162"/>
+      <c r="C1164" s="163"/>
+      <c r="D1164" s="164"/>
+      <c r="E1164" s="164"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1165" s="69">
@@ -14035,9 +14565,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="161"/>
-      <c r="D1181" s="162"/>
-      <c r="E1181" s="162"/>
+      <c r="C1181" s="163"/>
+      <c r="D1181" s="164"/>
+      <c r="E1181" s="164"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A1182" s="69">
@@ -14188,9 +14718,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="161"/>
-      <c r="D1198" s="162"/>
-      <c r="E1198" s="162"/>
+      <c r="C1198" s="163"/>
+      <c r="D1198" s="164"/>
+      <c r="E1198" s="164"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1199" s="69">
@@ -14341,9 +14871,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="161"/>
-      <c r="D1215" s="162"/>
-      <c r="E1215" s="162"/>
+      <c r="C1215" s="163"/>
+      <c r="D1215" s="164"/>
+      <c r="E1215" s="164"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1216" s="69">
@@ -14494,9 +15024,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="161"/>
-      <c r="D1232" s="162"/>
-      <c r="E1232" s="162"/>
+      <c r="C1232" s="163"/>
+      <c r="D1232" s="164"/>
+      <c r="E1232" s="164"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1233" s="69">
@@ -14647,9 +15177,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="161"/>
-      <c r="D1249" s="162"/>
-      <c r="E1249" s="162"/>
+      <c r="C1249" s="163"/>
+      <c r="D1249" s="164"/>
+      <c r="E1249" s="164"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1250" s="69">
@@ -14800,9 +15330,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="161"/>
-      <c r="D1266" s="162"/>
-      <c r="E1266" s="162"/>
+      <c r="C1266" s="163"/>
+      <c r="D1266" s="164"/>
+      <c r="E1266" s="164"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1267" s="69">
@@ -14953,9 +15483,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="161"/>
-      <c r="D1283" s="162"/>
-      <c r="E1283" s="162"/>
+      <c r="C1283" s="163"/>
+      <c r="D1283" s="164"/>
+      <c r="E1283" s="164"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1284" s="69">
@@ -15106,9 +15636,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="161"/>
-      <c r="D1300" s="162"/>
-      <c r="E1300" s="162"/>
+      <c r="C1300" s="163"/>
+      <c r="D1300" s="164"/>
+      <c r="E1300" s="164"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1301" s="69">
@@ -15259,9 +15789,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="161"/>
-      <c r="D1317" s="162"/>
-      <c r="E1317" s="162"/>
+      <c r="C1317" s="163"/>
+      <c r="D1317" s="164"/>
+      <c r="E1317" s="164"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1318" s="69">
@@ -15412,9 +15942,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="161"/>
-      <c r="D1334" s="162"/>
-      <c r="E1334" s="162"/>
+      <c r="C1334" s="163"/>
+      <c r="D1334" s="164"/>
+      <c r="E1334" s="164"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1335" s="69">
@@ -15565,9 +16095,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="161"/>
-      <c r="D1351" s="162"/>
-      <c r="E1351" s="162"/>
+      <c r="C1351" s="163"/>
+      <c r="D1351" s="164"/>
+      <c r="E1351" s="164"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1352" s="69">
@@ -15718,18 +16248,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="173"/>
-      <c r="D1368" s="174"/>
-      <c r="E1368" s="174"/>
+      <c r="C1368" s="175"/>
+      <c r="D1368" s="176"/>
+      <c r="E1368" s="176"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="161"/>
-      <c r="D1369" s="162"/>
-      <c r="E1369" s="162"/>
+      <c r="C1369" s="163"/>
+      <c r="D1369" s="164"/>
+      <c r="E1369" s="164"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1370" s="74">
@@ -15880,9 +16410,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="163"/>
-      <c r="D1386" s="164"/>
-      <c r="E1386" s="164"/>
+      <c r="C1386" s="165"/>
+      <c r="D1386" s="166"/>
+      <c r="E1386" s="166"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1387" s="74">
@@ -16033,9 +16563,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="161"/>
-      <c r="D1403" s="162"/>
-      <c r="E1403" s="162"/>
+      <c r="C1403" s="163"/>
+      <c r="D1403" s="164"/>
+      <c r="E1403" s="164"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1404" s="74">
@@ -16186,9 +16716,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="161"/>
-      <c r="D1420" s="162"/>
-      <c r="E1420" s="162"/>
+      <c r="C1420" s="163"/>
+      <c r="D1420" s="164"/>
+      <c r="E1420" s="164"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1421" s="74">
@@ -16339,9 +16869,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="161"/>
-      <c r="D1437" s="162"/>
-      <c r="E1437" s="162"/>
+      <c r="C1437" s="163"/>
+      <c r="D1437" s="164"/>
+      <c r="E1437" s="164"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1438" s="74">
@@ -16492,9 +17022,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="161"/>
-      <c r="D1454" s="162"/>
-      <c r="E1454" s="162"/>
+      <c r="C1454" s="163"/>
+      <c r="D1454" s="164"/>
+      <c r="E1454" s="164"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1455" s="74">
@@ -16645,9 +17175,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="161"/>
-      <c r="D1471" s="162"/>
-      <c r="E1471" s="162"/>
+      <c r="C1471" s="163"/>
+      <c r="D1471" s="164"/>
+      <c r="E1471" s="164"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1472" s="74">
@@ -16798,9 +17328,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="161"/>
-      <c r="D1488" s="162"/>
-      <c r="E1488" s="162"/>
+      <c r="C1488" s="163"/>
+      <c r="D1488" s="164"/>
+      <c r="E1488" s="164"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1489" s="74">
@@ -16951,9 +17481,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="161"/>
-      <c r="D1505" s="162"/>
-      <c r="E1505" s="162"/>
+      <c r="C1505" s="163"/>
+      <c r="D1505" s="164"/>
+      <c r="E1505" s="164"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1506" s="74">
@@ -17104,9 +17634,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="161"/>
-      <c r="D1522" s="162"/>
-      <c r="E1522" s="162"/>
+      <c r="C1522" s="163"/>
+      <c r="D1522" s="164"/>
+      <c r="E1522" s="164"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1523" s="74">
@@ -17257,9 +17787,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="161"/>
-      <c r="D1539" s="162"/>
-      <c r="E1539" s="162"/>
+      <c r="C1539" s="163"/>
+      <c r="D1539" s="164"/>
+      <c r="E1539" s="164"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1540" s="74">
@@ -17410,9 +17940,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="161"/>
-      <c r="D1556" s="162"/>
-      <c r="E1556" s="162"/>
+      <c r="C1556" s="163"/>
+      <c r="D1556" s="164"/>
+      <c r="E1556" s="164"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1557" s="74">
@@ -17563,9 +18093,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="161"/>
-      <c r="D1573" s="162"/>
-      <c r="E1573" s="162"/>
+      <c r="C1573" s="163"/>
+      <c r="D1573" s="164"/>
+      <c r="E1573" s="164"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1574" s="74">
@@ -17716,9 +18246,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="161"/>
-      <c r="D1590" s="162"/>
-      <c r="E1590" s="162"/>
+      <c r="C1590" s="163"/>
+      <c r="D1590" s="164"/>
+      <c r="E1590" s="164"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1591" s="74">
@@ -17869,9 +18399,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="161"/>
-      <c r="D1607" s="162"/>
-      <c r="E1607" s="162"/>
+      <c r="C1607" s="163"/>
+      <c r="D1607" s="164"/>
+      <c r="E1607" s="164"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1608" s="74">
@@ -18022,9 +18552,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="161"/>
-      <c r="D1624" s="162"/>
-      <c r="E1624" s="162"/>
+      <c r="C1624" s="163"/>
+      <c r="D1624" s="164"/>
+      <c r="E1624" s="164"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1625" s="74">
@@ -18175,18 +18705,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="175"/>
-      <c r="D1641" s="176"/>
-      <c r="E1641" s="176"/>
+      <c r="C1641" s="177"/>
+      <c r="D1641" s="178"/>
+      <c r="E1641" s="178"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="161"/>
-      <c r="D1642" s="162"/>
-      <c r="E1642" s="162"/>
+      <c r="C1642" s="163"/>
+      <c r="D1642" s="164"/>
+      <c r="E1642" s="164"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1643" s="79">
@@ -18337,9 +18867,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="163"/>
-      <c r="D1659" s="164"/>
-      <c r="E1659" s="164"/>
+      <c r="C1659" s="165"/>
+      <c r="D1659" s="166"/>
+      <c r="E1659" s="166"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1660" s="79">
@@ -18490,9 +19020,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="161"/>
-      <c r="D1676" s="162"/>
-      <c r="E1676" s="162"/>
+      <c r="C1676" s="163"/>
+      <c r="D1676" s="164"/>
+      <c r="E1676" s="164"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1677" s="79">
@@ -18643,9 +19173,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="161"/>
-      <c r="D1693" s="162"/>
-      <c r="E1693" s="162"/>
+      <c r="C1693" s="163"/>
+      <c r="D1693" s="164"/>
+      <c r="E1693" s="164"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1694" s="79">
@@ -18796,9 +19326,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="161"/>
-      <c r="D1710" s="162"/>
-      <c r="E1710" s="162"/>
+      <c r="C1710" s="163"/>
+      <c r="D1710" s="164"/>
+      <c r="E1710" s="164"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1711" s="79">
@@ -18949,9 +19479,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="161"/>
-      <c r="D1727" s="162"/>
-      <c r="E1727" s="162"/>
+      <c r="C1727" s="163"/>
+      <c r="D1727" s="164"/>
+      <c r="E1727" s="164"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1728" s="79">
@@ -19102,9 +19632,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="161"/>
-      <c r="D1744" s="162"/>
-      <c r="E1744" s="162"/>
+      <c r="C1744" s="163"/>
+      <c r="D1744" s="164"/>
+      <c r="E1744" s="164"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1745" s="79">
@@ -19255,9 +19785,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="161"/>
-      <c r="D1761" s="162"/>
-      <c r="E1761" s="162"/>
+      <c r="C1761" s="163"/>
+      <c r="D1761" s="164"/>
+      <c r="E1761" s="164"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1762" s="79">
@@ -19408,9 +19938,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="161"/>
-      <c r="D1778" s="162"/>
-      <c r="E1778" s="162"/>
+      <c r="C1778" s="163"/>
+      <c r="D1778" s="164"/>
+      <c r="E1778" s="164"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1779" s="79">
@@ -19561,9 +20091,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="161"/>
-      <c r="D1795" s="162"/>
-      <c r="E1795" s="162"/>
+      <c r="C1795" s="163"/>
+      <c r="D1795" s="164"/>
+      <c r="E1795" s="164"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1796" s="79">
@@ -19714,9 +20244,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="161"/>
-      <c r="D1812" s="162"/>
-      <c r="E1812" s="162"/>
+      <c r="C1812" s="163"/>
+      <c r="D1812" s="164"/>
+      <c r="E1812" s="164"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1813" s="79">
@@ -19867,9 +20397,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="161"/>
-      <c r="D1829" s="162"/>
-      <c r="E1829" s="162"/>
+      <c r="C1829" s="163"/>
+      <c r="D1829" s="164"/>
+      <c r="E1829" s="164"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1830" s="79">
@@ -20020,9 +20550,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="161"/>
-      <c r="D1846" s="162"/>
-      <c r="E1846" s="162"/>
+      <c r="C1846" s="163"/>
+      <c r="D1846" s="164"/>
+      <c r="E1846" s="164"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1847" s="79">
@@ -20173,9 +20703,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="161"/>
-      <c r="D1863" s="162"/>
-      <c r="E1863" s="162"/>
+      <c r="C1863" s="163"/>
+      <c r="D1863" s="164"/>
+      <c r="E1863" s="164"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1864" s="79">
@@ -20326,9 +20856,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="161"/>
-      <c r="D1880" s="162"/>
-      <c r="E1880" s="162"/>
+      <c r="C1880" s="163"/>
+      <c r="D1880" s="164"/>
+      <c r="E1880" s="164"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1881" s="79">
@@ -20479,9 +21009,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="161"/>
-      <c r="D1897" s="162"/>
-      <c r="E1897" s="162"/>
+      <c r="C1897" s="163"/>
+      <c r="D1897" s="164"/>
+      <c r="E1897" s="164"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1898" s="79">
@@ -20632,18 +21162,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="177"/>
-      <c r="D1914" s="178"/>
-      <c r="E1914" s="178"/>
+      <c r="C1914" s="179"/>
+      <c r="D1914" s="180"/>
+      <c r="E1914" s="180"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="161"/>
-      <c r="D1915" s="162"/>
-      <c r="E1915" s="162"/>
+      <c r="C1915" s="163"/>
+      <c r="D1915" s="164"/>
+      <c r="E1915" s="164"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1916" s="84">
@@ -20794,9 +21324,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="163"/>
-      <c r="D1932" s="164"/>
-      <c r="E1932" s="164"/>
+      <c r="C1932" s="165"/>
+      <c r="D1932" s="166"/>
+      <c r="E1932" s="166"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1933" s="84">
@@ -20947,9 +21477,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="161"/>
-      <c r="D1949" s="162"/>
-      <c r="E1949" s="162"/>
+      <c r="C1949" s="163"/>
+      <c r="D1949" s="164"/>
+      <c r="E1949" s="164"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1950" s="84">
@@ -21100,9 +21630,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="161"/>
-      <c r="D1966" s="162"/>
-      <c r="E1966" s="162"/>
+      <c r="C1966" s="163"/>
+      <c r="D1966" s="164"/>
+      <c r="E1966" s="164"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1967" s="84">
@@ -21253,9 +21783,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="161"/>
-      <c r="D1983" s="162"/>
-      <c r="E1983" s="162"/>
+      <c r="C1983" s="163"/>
+      <c r="D1983" s="164"/>
+      <c r="E1983" s="164"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1984" s="84">
@@ -21406,9 +21936,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="161"/>
-      <c r="D2000" s="162"/>
-      <c r="E2000" s="162"/>
+      <c r="C2000" s="163"/>
+      <c r="D2000" s="164"/>
+      <c r="E2000" s="164"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2001" s="84">
@@ -21559,9 +22089,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="161"/>
-      <c r="D2017" s="162"/>
-      <c r="E2017" s="162"/>
+      <c r="C2017" s="163"/>
+      <c r="D2017" s="164"/>
+      <c r="E2017" s="164"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2018" s="84">
@@ -21712,9 +22242,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="161"/>
-      <c r="D2034" s="162"/>
-      <c r="E2034" s="162"/>
+      <c r="C2034" s="163"/>
+      <c r="D2034" s="164"/>
+      <c r="E2034" s="164"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2035" s="84">
@@ -21865,9 +22395,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="161"/>
-      <c r="D2051" s="162"/>
-      <c r="E2051" s="162"/>
+      <c r="C2051" s="163"/>
+      <c r="D2051" s="164"/>
+      <c r="E2051" s="164"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2052" s="84">
@@ -22018,9 +22548,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="161"/>
-      <c r="D2068" s="162"/>
-      <c r="E2068" s="162"/>
+      <c r="C2068" s="163"/>
+      <c r="D2068" s="164"/>
+      <c r="E2068" s="164"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2069" s="84">
@@ -22171,9 +22701,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="161"/>
-      <c r="D2085" s="162"/>
-      <c r="E2085" s="162"/>
+      <c r="C2085" s="163"/>
+      <c r="D2085" s="164"/>
+      <c r="E2085" s="164"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2086" s="84">
@@ -22324,9 +22854,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="161"/>
-      <c r="D2102" s="162"/>
-      <c r="E2102" s="162"/>
+      <c r="C2102" s="163"/>
+      <c r="D2102" s="164"/>
+      <c r="E2102" s="164"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2103" s="84">
@@ -22477,9 +23007,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="161"/>
-      <c r="D2119" s="162"/>
-      <c r="E2119" s="162"/>
+      <c r="C2119" s="163"/>
+      <c r="D2119" s="164"/>
+      <c r="E2119" s="164"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2120" s="84">
@@ -22630,9 +23160,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="161"/>
-      <c r="D2136" s="162"/>
-      <c r="E2136" s="162"/>
+      <c r="C2136" s="163"/>
+      <c r="D2136" s="164"/>
+      <c r="E2136" s="164"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2137" s="84">
@@ -22783,9 +23313,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="161"/>
-      <c r="D2153" s="162"/>
-      <c r="E2153" s="162"/>
+      <c r="C2153" s="163"/>
+      <c r="D2153" s="164"/>
+      <c r="E2153" s="164"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2154" s="84">
@@ -22936,9 +23466,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="161"/>
-      <c r="D2170" s="162"/>
-      <c r="E2170" s="162"/>
+      <c r="C2170" s="163"/>
+      <c r="D2170" s="164"/>
+      <c r="E2170" s="164"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2171" s="84">
@@ -23224,7 +23754,7 @@
     <mergeCell ref="C72:E72"/>
     <mergeCell ref="C208:E208"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -23249,51 +23779,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="185" t="s">
+      <c r="A1" s="187" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="185"/>
-      <c r="C1" s="185"/>
-      <c r="D1" s="185"/>
-      <c r="E1" s="185"/>
-      <c r="F1" s="185"/>
-      <c r="G1" s="185"/>
-      <c r="H1" s="185"/>
-      <c r="I1" s="185"/>
-      <c r="J1" s="185"/>
-      <c r="K1" s="185"/>
-      <c r="L1" s="185"/>
+      <c r="B1" s="187"/>
+      <c r="C1" s="187"/>
+      <c r="D1" s="187"/>
+      <c r="E1" s="187"/>
+      <c r="F1" s="187"/>
+      <c r="G1" s="187"/>
+      <c r="H1" s="187"/>
+      <c r="I1" s="187"/>
+      <c r="J1" s="187"/>
+      <c r="K1" s="187"/>
+      <c r="L1" s="187"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="182" t="s">
+      <c r="A2" s="184" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="183"/>
-      <c r="C2" s="183"/>
-      <c r="D2" s="183"/>
-      <c r="E2" s="183"/>
-      <c r="F2" s="183"/>
-      <c r="G2" s="183"/>
-      <c r="H2" s="183"/>
-      <c r="I2" s="183"/>
-      <c r="J2" s="183"/>
-      <c r="K2" s="183"/>
-      <c r="L2" s="184"/>
+      <c r="B2" s="185"/>
+      <c r="C2" s="185"/>
+      <c r="D2" s="185"/>
+      <c r="E2" s="185"/>
+      <c r="F2" s="185"/>
+      <c r="G2" s="185"/>
+      <c r="H2" s="185"/>
+      <c r="I2" s="185"/>
+      <c r="J2" s="185"/>
+      <c r="K2" s="185"/>
+      <c r="L2" s="186"/>
     </row>
     <row r="3" spans="1:12" s="31" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="179" t="s">
+      <c r="A3" s="181" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="180"/>
-      <c r="C3" s="180"/>
-      <c r="D3" s="180"/>
-      <c r="E3" s="180"/>
-      <c r="F3" s="180"/>
-      <c r="G3" s="180"/>
-      <c r="H3" s="180"/>
-      <c r="I3" s="180"/>
-      <c r="J3" s="180"/>
-      <c r="K3" s="181"/>
+      <c r="B3" s="182"/>
+      <c r="C3" s="182"/>
+      <c r="D3" s="182"/>
+      <c r="E3" s="182"/>
+      <c r="F3" s="182"/>
+      <c r="G3" s="182"/>
+      <c r="H3" s="182"/>
+      <c r="I3" s="182"/>
+      <c r="J3" s="182"/>
+      <c r="K3" s="183"/>
     </row>
     <row r="4" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="28" t="s">
@@ -23510,19 +24040,19 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="179" t="s">
+      <c r="A20" s="181" t="s">
         <v>166</v>
       </c>
-      <c r="B20" s="180"/>
-      <c r="C20" s="180"/>
-      <c r="D20" s="180"/>
-      <c r="E20" s="180"/>
-      <c r="F20" s="180"/>
-      <c r="G20" s="180"/>
-      <c r="H20" s="180"/>
-      <c r="I20" s="180"/>
-      <c r="J20" s="180"/>
-      <c r="K20" s="181"/>
+      <c r="B20" s="182"/>
+      <c r="C20" s="182"/>
+      <c r="D20" s="182"/>
+      <c r="E20" s="182"/>
+      <c r="F20" s="182"/>
+      <c r="G20" s="182"/>
+      <c r="H20" s="182"/>
+      <c r="I20" s="182"/>
+      <c r="J20" s="182"/>
+      <c r="K20" s="183"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="28" t="s">
@@ -23739,19 +24269,19 @@
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="179" t="s">
+      <c r="A37" s="181" t="s">
         <v>167</v>
       </c>
-      <c r="B37" s="180"/>
-      <c r="C37" s="180"/>
-      <c r="D37" s="180"/>
-      <c r="E37" s="180"/>
-      <c r="F37" s="180"/>
-      <c r="G37" s="180"/>
-      <c r="H37" s="180"/>
-      <c r="I37" s="180"/>
-      <c r="J37" s="180"/>
-      <c r="K37" s="181"/>
+      <c r="B37" s="182"/>
+      <c r="C37" s="182"/>
+      <c r="D37" s="182"/>
+      <c r="E37" s="182"/>
+      <c r="F37" s="182"/>
+      <c r="G37" s="182"/>
+      <c r="H37" s="182"/>
+      <c r="I37" s="182"/>
+      <c r="J37" s="182"/>
+      <c r="K37" s="183"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="28" t="s">
@@ -23975,7 +24505,7 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A20:K20"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -24009,28 +24539,28 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="186"/>
+      <c r="A3" s="188"/>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="187"/>
+      <c r="A4" s="189"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="187"/>
+      <c r="A5" s="189"/>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="187"/>
+      <c r="A6" s="189"/>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="187"/>
+      <c r="A7" s="189"/>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="187"/>
+      <c r="A8" s="189"/>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="187"/>
+      <c r="A9" s="189"/>
     </row>
     <row r="10" spans="1:1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="188"/>
+      <c r="A10" s="190"/>
     </row>
     <row r="11" spans="1:1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
@@ -24186,7 +24716,7 @@
   <mergeCells count="1">
     <mergeCell ref="A3:A10"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -24213,10 +24743,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="189" t="s">
+      <c r="B1" s="191" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="190"/>
+      <c r="C1" s="192"/>
       <c r="D1" s="92"/>
       <c r="E1" s="32"/>
     </row>
@@ -24227,7 +24757,7 @@
       <c r="E2" s="119"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="191" t="s">
+      <c r="A3" s="193" t="s">
         <v>205</v>
       </c>
       <c r="B3" s="131" t="s">
@@ -24241,7 +24771,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="192"/>
+      <c r="A4" s="194"/>
       <c r="B4" s="128" t="s">
         <v>159</v>
       </c>
@@ -24253,7 +24783,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="192"/>
+      <c r="A5" s="194"/>
       <c r="B5" s="128" t="s">
         <v>160</v>
       </c>
@@ -24262,31 +24792,31 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="192"/>
+      <c r="A6" s="194"/>
       <c r="B6" s="139" t="s">
         <v>207</v>
       </c>
       <c r="C6" s="134">
         <f>FrameCounts!H2</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="192"/>
+      <c r="A7" s="194"/>
       <c r="B7" s="128" t="s">
         <v>173</v>
       </c>
       <c r="C7" s="135">
         <f>C6/60</f>
-        <v>0</v>
+        <v>3.3333333333333333E-2</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="192"/>
+      <c r="A8" s="194"/>
       <c r="B8" s="128" t="s">
         <v>174</v>
       </c>
@@ -24295,7 +24825,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="193"/>
+      <c r="A9" s="195"/>
       <c r="B9" s="136" t="s">
         <v>161</v>
       </c>
@@ -24310,7 +24840,7 @@
       <c r="E10" s="94"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="191" t="s">
+      <c r="A11" s="193" t="s">
         <v>206</v>
       </c>
       <c r="B11" s="131" t="s">
@@ -24324,7 +24854,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="192"/>
+      <c r="A12" s="194"/>
       <c r="B12" s="128" t="s">
         <v>159</v>
       </c>
@@ -24336,7 +24866,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="192"/>
+      <c r="A13" s="194"/>
       <c r="B13" s="128" t="s">
         <v>160</v>
       </c>
@@ -24345,7 +24875,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="192"/>
+      <c r="A14" s="194"/>
       <c r="B14" s="139" t="s">
         <v>207</v>
       </c>
@@ -24357,7 +24887,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="192"/>
+      <c r="A15" s="194"/>
       <c r="B15" s="128" t="s">
         <v>173</v>
       </c>
@@ -24369,7 +24899,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="192"/>
+      <c r="A16" s="194"/>
       <c r="B16" s="128" t="s">
         <v>174</v>
       </c>
@@ -24378,7 +24908,7 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="193"/>
+      <c r="A17" s="195"/>
       <c r="B17" s="136" t="s">
         <v>161</v>
       </c>
@@ -24393,7 +24923,7 @@
       <c r="E18" s="94"/>
     </row>
     <row r="19" spans="1:5" collapsed="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="191" t="s">
+      <c r="A19" s="193" t="s">
         <v>206</v>
       </c>
       <c r="B19" s="131" t="s">
@@ -24402,7 +24932,7 @@
       <c r="C19" s="130"/>
     </row>
     <row r="20" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="192"/>
+      <c r="A20" s="194"/>
       <c r="B20" s="128" t="s">
         <v>159</v>
       </c>
@@ -24412,14 +24942,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="192"/>
+      <c r="A21" s="194"/>
       <c r="B21" s="128" t="s">
         <v>160</v>
       </c>
       <c r="C21" s="133"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="192"/>
+      <c r="A22" s="194"/>
       <c r="B22" s="139" t="s">
         <v>207</v>
       </c>
@@ -24429,7 +24959,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="192"/>
+      <c r="A23" s="194"/>
       <c r="B23" s="128" t="s">
         <v>173</v>
       </c>
@@ -24439,14 +24969,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="192"/>
+      <c r="A24" s="194"/>
       <c r="B24" s="128" t="s">
         <v>174</v>
       </c>
       <c r="C24" s="132"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="193"/>
+      <c r="A25" s="195"/>
       <c r="B25" s="136" t="s">
         <v>161</v>
       </c>
@@ -24459,7 +24989,7 @@
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A19:A25"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -24481,147 +25011,147 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33" x14ac:dyDescent="0.45">
-      <c r="A1" s="204" t="s">
+      <c r="A1" s="206" t="s">
         <v>187</v>
       </c>
-      <c r="B1" s="205"/>
+      <c r="B1" s="207"/>
       <c r="C1" s="118"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="210" t="s">
+      <c r="A2" s="212" t="s">
         <v>186</v>
       </c>
-      <c r="B2" s="211"/>
+      <c r="B2" s="213"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="212" t="s">
+      <c r="A3" s="214" t="s">
         <v>188</v>
       </c>
-      <c r="B3" s="211"/>
+      <c r="B3" s="213"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="208"/>
-      <c r="B4" s="209"/>
+      <c r="A4" s="210"/>
+      <c r="B4" s="211"/>
       <c r="C4" s="120"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="206" t="s">
+      <c r="A5" s="208" t="s">
         <v>197</v>
       </c>
-      <c r="B5" s="207"/>
+      <c r="B5" s="209"/>
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="198" t="s">
+      <c r="A7" s="200" t="s">
         <v>189</v>
       </c>
-      <c r="B7" s="199"/>
+      <c r="B7" s="201"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="200" t="s">
+      <c r="A9" s="202" t="s">
         <v>190</v>
       </c>
-      <c r="B9" s="201"/>
+      <c r="B9" s="203"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="202"/>
-      <c r="B10" s="203"/>
+      <c r="A10" s="204"/>
+      <c r="B10" s="205"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="194" t="s">
+      <c r="A11" s="196" t="s">
         <v>191</v>
       </c>
-      <c r="B11" s="195"/>
+      <c r="B11" s="197"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="194" t="s">
+      <c r="A12" s="196" t="s">
         <v>192</v>
       </c>
-      <c r="B12" s="195"/>
+      <c r="B12" s="197"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="194" t="s">
+      <c r="A13" s="196" t="s">
         <v>193</v>
       </c>
-      <c r="B13" s="195"/>
+      <c r="B13" s="197"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="194" t="s">
+      <c r="A14" s="196" t="s">
         <v>194</v>
       </c>
-      <c r="B14" s="195"/>
+      <c r="B14" s="197"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="194" t="s">
+      <c r="A15" s="196" t="s">
         <v>195</v>
       </c>
-      <c r="B15" s="195"/>
+      <c r="B15" s="197"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="194" t="s">
+      <c r="A16" s="196" t="s">
         <v>196</v>
       </c>
-      <c r="B16" s="195"/>
+      <c r="B16" s="197"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="196" t="s">
+      <c r="A17" s="198" t="s">
         <v>198</v>
       </c>
-      <c r="B17" s="197"/>
+      <c r="B17" s="199"/>
     </row>
     <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="198" t="s">
+      <c r="A19" s="200" t="s">
         <v>200</v>
       </c>
-      <c r="B19" s="199"/>
+      <c r="B19" s="201"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="200" t="s">
+      <c r="A21" s="202" t="s">
         <v>201</v>
       </c>
-      <c r="B21" s="201"/>
+      <c r="B21" s="203"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="202"/>
-      <c r="B22" s="203"/>
+      <c r="A22" s="204"/>
+      <c r="B22" s="205"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="194" t="s">
+      <c r="A23" s="196" t="s">
         <v>202</v>
       </c>
-      <c r="B23" s="195"/>
+      <c r="B23" s="197"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="194"/>
-      <c r="B24" s="195"/>
+      <c r="A24" s="196"/>
+      <c r="B24" s="197"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="194" t="s">
+      <c r="A25" s="196" t="s">
         <v>203</v>
       </c>
-      <c r="B25" s="195"/>
+      <c r="B25" s="197"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="194" t="s">
+      <c r="A26" s="196" t="s">
         <v>204</v>
       </c>
-      <c r="B26" s="195"/>
+      <c r="B26" s="197"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="196"/>
-      <c r="B27" s="197"/>
+      <c r="A27" s="198"/>
+      <c r="B27" s="199"/>
     </row>
   </sheetData>
   <mergeCells count="23">

</xml_diff>